<commit_message>
Table numbers added to ANOVA.tables...xlsx
</commit_message>
<xml_diff>
--- a/tables_figs/anova_tables_figs/ANOVA.tables.SSB.F.Catch.xlsx
+++ b/tables_figs/anova_tables_figs/ANOVA.tables.SSB.F.Catch.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liz.brooks\liz\Docs\Requests\FY_2020\PlanB\report\anova_output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liz.brooks\liz\Github\IBMWG\tables_figs\anova_tables_figs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15340" windowHeight="6850" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15340" windowHeight="6850"/>
   </bookViews>
   <sheets>
     <sheet name="SSB.frac.explained.ANOVA" sheetId="1" r:id="rId1"/>
@@ -71,18 +71,9 @@
     <t>SS.frac.explained</t>
   </si>
   <si>
-    <t>Table 5.x.anova.ssb</t>
-  </si>
-  <si>
     <t>Factor</t>
   </si>
   <si>
-    <t>Table 5.x.anova.f</t>
-  </si>
-  <si>
-    <t>Table 5.x.anova.catch</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -207,6 +198,15 @@
   </si>
   <si>
     <t>time horizon consistently explained the largest fraction (except for the two catch curve methods, where Fhist most important)</t>
+  </si>
+  <si>
+    <t>Table 5.3.anova.catch</t>
+  </si>
+  <si>
+    <t>Table 5.2.anova.f</t>
+  </si>
+  <si>
+    <t>Table 5.1.anova.ssb</t>
   </si>
 </sst>
 </file>
@@ -1222,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1237,30 +1237,30 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="F3" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>37</v>
-      </c>
       <c r="G3" s="20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>0</v>
@@ -1269,19 +1269,19 @@
         <v>3</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K3" s="20" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1328,10 +1328,10 @@
         <v>0.42699999999999999</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1354,16 +1354,16 @@
         <v>2.4E-2</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I5" s="6">
         <v>1.9E-2</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K5" s="6">
         <v>5.0000000000000001E-3</v>
@@ -1378,10 +1378,10 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="Q5" s="18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -1389,49 +1389,49 @@
         <v>6</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J6" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q6" s="19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -1442,7 +1442,7 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" s="6">
         <v>1.6E-2</v>
@@ -1478,10 +1478,10 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -1492,25 +1492,25 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F8" s="5">
         <v>0.1</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J8" s="6">
         <v>0.20799999999999999</v>
@@ -1525,13 +1525,13 @@
         <v>0.20200000000000001</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
@@ -1542,13 +1542,13 @@
         <v>1.6E-2</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F9" s="6">
         <v>1.0999999999999999E-2</v>
@@ -1560,7 +1560,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J9" s="6">
         <v>4.1000000000000002E-2</v>
@@ -1578,10 +1578,10 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -1589,49 +1589,49 @@
         <v>10</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q10" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="R10" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
@@ -1639,10 +1639,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" s="6">
         <v>0.01</v>
@@ -1651,31 +1651,31 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I11" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
@@ -1683,19 +1683,19 @@
         <v>12</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G12" s="6">
         <v>8.9999999999999993E-3</v>
@@ -1704,19 +1704,19 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N12" s="6">
         <v>2.1000000000000001E-2</v>
@@ -1730,10 +1730,10 @@
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E13" s="6">
         <v>5.0000000000000001E-3</v>
@@ -1742,10 +1742,10 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I13" s="6">
         <v>5.0000000000000001E-3</v>
@@ -1771,43 +1771,43 @@
         <v>14</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
@@ -1856,37 +1856,37 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1906,8 +1906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1922,7 +1922,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -1930,25 +1930,25 @@
     </row>
     <row r="3" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="F3" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>37</v>
-      </c>
       <c r="G3" s="20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>0</v>
@@ -1957,25 +1957,25 @@
         <v>3</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K3" s="20" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -2022,10 +2022,10 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="Q4" s="18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="R4" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -2039,10 +2039,10 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5" s="21">
         <v>1.9E-2</v>
@@ -2054,7 +2054,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J5" s="6">
         <v>4.2000000000000003E-2</v>
@@ -2069,13 +2069,13 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="N5" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -2086,28 +2086,28 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D6" s="21">
         <v>2.7E-2</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" s="21">
         <v>1.6E-2</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H6" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K6" s="6">
         <v>0.01</v>
@@ -2116,16 +2116,16 @@
         <v>1.4E-2</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N6" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -2136,7 +2136,7 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="21">
         <v>1.4E-2</v>
@@ -2172,10 +2172,10 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -2189,43 +2189,43 @@
         <v>1.4E-2</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E8" s="23">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I8" s="5">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M8" s="6">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="N8" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Q8" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
@@ -2239,28 +2239,28 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F9" s="21">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L9" s="6">
         <v>1.0999999999999999E-2</v>
@@ -2269,13 +2269,13 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="N9" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Q9" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="R9" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -2283,19 +2283,19 @@
         <v>10</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" s="21">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G10" s="5">
         <v>7.1999999999999995E-2</v>
@@ -2304,7 +2304,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J10" s="6">
         <v>1.2999999999999999E-2</v>
@@ -2313,7 +2313,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M10" s="6">
         <v>1.4999999999999999E-2</v>
@@ -2330,25 +2330,25 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F11" s="21">
         <v>3.1E-2</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J11" s="6">
         <v>1.2E-2</v>
@@ -2371,43 +2371,43 @@
         <v>12</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" s="21">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E12" s="23">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I12" s="5">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
@@ -2418,40 +2418,40 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F13" s="21">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L13" s="6">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
@@ -2459,43 +2459,43 @@
         <v>14</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
@@ -2544,37 +2544,37 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2602,8 +2602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2618,30 +2618,30 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="F3" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>37</v>
-      </c>
       <c r="G3" s="20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>0</v>
@@ -2650,25 +2650,25 @@
         <v>3</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K3" s="20" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -2712,13 +2712,13 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="N4" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Q4" s="18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="R4" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -2738,7 +2738,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G5" s="6">
         <v>0.04</v>
@@ -2756,19 +2756,19 @@
         <v>0.126</v>
       </c>
       <c r="L5" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N5" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -2776,49 +2776,49 @@
         <v>6</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G6" s="6">
         <v>0.01</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J6" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -2829,25 +2829,25 @@
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F7" s="6">
         <v>0.127</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J7" s="6">
         <v>0.04</v>
@@ -2862,13 +2862,13 @@
         <v>0.108</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -2879,7 +2879,7 @@
         <v>0.19900000000000001</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D8" s="6">
         <v>0.23599999999999999</v>
@@ -2915,10 +2915,10 @@
         <v>0.105</v>
       </c>
       <c r="Q8" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
@@ -2926,7 +2926,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="6">
         <v>4.9000000000000002E-2</v>
@@ -2938,7 +2938,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G9" s="5">
         <v>9.6000000000000002E-2</v>
@@ -2956,19 +2956,19 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N9" s="5">
         <v>6.2E-2</v>
       </c>
       <c r="Q9" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="R9" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -2982,7 +2982,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" s="6">
         <v>1.4E-2</v>
@@ -2991,25 +2991,25 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I10" s="6">
         <v>1.4E-2</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L10" s="6">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N10" s="6">
         <v>1.7000000000000001E-2</v>
@@ -3020,43 +3020,43 @@
         <v>11</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N11" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
@@ -3064,7 +3064,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5">
         <v>6.0999999999999999E-2</v>
@@ -3076,7 +3076,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G12" s="6">
         <v>0.14299999999999999</v>
@@ -3094,10 +3094,10 @@
         <v>1.2E-2</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N12" s="5">
         <v>7.2999999999999995E-2</v>
@@ -3108,40 +3108,40 @@
         <v>13</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L13" s="6">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N13" s="6">
         <v>1.0999999999999999E-2</v>
@@ -3152,43 +3152,43 @@
         <v>14</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N14" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
@@ -3237,37 +3237,37 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>